<commit_message>
Inserting flexibility inputs, now need to add on the OF, main and plots
</commit_message>
<xml_diff>
--- a/data/Loads/26h_BTA4_7.xlsx
+++ b/data/Loads/26h_BTA4_7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lorenzo.giannuzzo\PycharmProjects\BESS-Optimization\data\Loads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{755B13C4-1295-4004-A42E-3B34140CC1CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C482A75E-BF34-4EAA-BE80-C9F07B69F52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -454,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD8761"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A2:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,7 +482,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>44562</v>
+        <v>45431.916666666664</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -499,7 +499,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>44562</v>
+        <v>45431.958333333336</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -516,7 +516,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>44562</v>
+        <v>45432</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -533,7 +533,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>44562</v>
+        <v>45432.041666666664</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>44562</v>
+        <v>45432.08333321759</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -567,7 +567,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>44562</v>
+        <v>45432.124999826388</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -584,7 +584,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>44562</v>
+        <v>45432.166666435187</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -601,7 +601,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>44562</v>
+        <v>45432.208333043978</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>44562</v>
+        <v>45432.249999652777</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -635,7 +635,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>44562</v>
+        <v>45432.291666261575</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>44562</v>
+        <v>45432.333332870374</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -669,7 +669,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>44562</v>
+        <v>45432.374999479165</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -686,7 +686,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>44562</v>
+        <v>45432.416666087964</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -703,7 +703,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>44562</v>
+        <v>45432.458332696762</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -720,7 +720,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>44562</v>
+        <v>45432.499999305554</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -737,7 +737,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>44562</v>
+        <v>45432.541665914352</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -754,7 +754,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>44562</v>
+        <v>45432.583332523151</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -771,7 +771,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>44562</v>
+        <v>45432.624999131942</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -788,7 +788,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>44562</v>
+        <v>45432.66666574074</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -805,7 +805,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>44562</v>
+        <v>45432.708332349539</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -822,7 +822,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>44562</v>
+        <v>45432.74999895833</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -839,7 +839,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>44562</v>
+        <v>45432.791665567129</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -856,7 +856,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>44562</v>
+        <v>45432.833332175927</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -873,7 +873,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>44562</v>
+        <v>45432.874998784719</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -890,7 +890,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>44563</v>
+        <v>45432.916665393517</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -907,7 +907,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>44563</v>
+        <v>45432.958332002316</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -939,6 +939,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100FB9475D466104B4F8254900DD2928249" ma:contentTypeVersion="12" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="51bfdcbcfa4b53868757ab92efd2e4cf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73f032b1-d858-4e52-a112-ff8a449379e0" xmlns:ns3="2cf41f78-c934-4264-8805-5389acee063d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="af5ace7edf031339c2ec4586fdd3025f" ns2:_="" ns3:_="">
     <xsd:import namespace="73f032b1-d858-4e52-a112-ff8a449379e0"/>
@@ -1149,15 +1158,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA1B6BB8-FD2A-4AEA-B6AE-93A661D322ED}">
   <ds:schemaRefs>
@@ -1169,6 +1169,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60A95E8C-2DF0-417F-AE2A-4B76F2DB91C2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFF38105-3D33-41BD-B0FD-8B52FBC5D4A3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1185,12 +1193,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60A95E8C-2DF0-417F-AE2A-4B76F2DB91C2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>